<commit_message>
6 pin SH connector instead of two 4 pin SH connectors
</commit_message>
<xml_diff>
--- a/BOM MAIN BOARD.xlsx
+++ b/BOM MAIN BOARD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\braed\Documents\EAGLE\projects\SP Throttle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{914217FC-8C49-46BC-9D81-303F3E7BA5D4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B4EA28E-10A7-4805-8BA5-CA273F005A4D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7A6408F3-8FEB-416E-8A51-1ABFD5653230}"/>
+    <workbookView xWindow="2220" yWindow="2064" windowWidth="17280" windowHeight="9024" xr2:uid="{7A6408F3-8FEB-416E-8A51-1ABFD5653230}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="133">
   <si>
     <t>Qty</t>
   </si>
@@ -390,19 +390,46 @@
     <t>C5, C6, C7, C10, C11, C12, C14, C17</t>
   </si>
   <si>
-    <t>ESC, TELEM</t>
-  </si>
-  <si>
-    <t>BM04B-SRSS-TB(LF)(SN)</t>
-  </si>
-  <si>
-    <t>JST SH 1MM</t>
-  </si>
-  <si>
     <t>JST SH 1MM VERT</t>
   </si>
   <si>
-    <t>JST SH 4-PIN TO PREMIUM MALE HEA</t>
+    <t>J2</t>
+  </si>
+  <si>
+    <t>‎BM06B-SRSS-TB(LF)(SN)‎</t>
+  </si>
+  <si>
+    <t>JST SH 1MM 6 PIN</t>
+  </si>
+  <si>
+    <t>‎SSH-003T-P0.2</t>
+  </si>
+  <si>
+    <t>AWG28-08/F-1/300</t>
+  </si>
+  <si>
+    <t>SHR-06V-S</t>
+  </si>
+  <si>
+    <t>‎M20-1060400</t>
+  </si>
+  <si>
+    <t>M20-1160042‎</t>
+  </si>
+  <si>
+    <t>CONN SOCKET 28-32AWG CRIMP TIN</t>
+  </si>
+  <si>
+    <t>CBL RIBN 8COND 0.039 MULTI 5'</t>
+  </si>
+  <si>
+    <t>CONN HOUSING SH 6POS 1MM WHITE</t>
+  </si>
+  <si>
+    <t>CONN RCPT HSG 4POS 2.54MM</t>
+  </si>
+  <si>
+    <t>CONN SOCKET 22-30AWG CRIMP GOLD</t>
   </si>
 </sst>
 </file>
@@ -770,10 +797,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A2FCF1E-2965-4CA3-9C3D-EDB553ECE1A4}">
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1017,25 +1044,25 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B11" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="E11" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="D11" s="4" t="s">
+      <c r="F11" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="G11" s="4" t="s">
         <v>121</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -1511,23 +1538,58 @@
     </row>
     <row r="33" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="4">
+        <v>6</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="G33" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A34" s="4">
+        <v>1</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="G34" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A35" s="4">
+        <v>1</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="G35" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A36" s="4">
         <v>2</v>
       </c>
-      <c r="F33" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="G33">
-        <v>4209</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="F34" s="2"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="F35" s="2"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="F36" s="2"/>
+      <c r="F36" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="G36" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A37" s="4">
+        <v>8</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="G37" t="s">
+        <v>127</v>
+      </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G32">

</xml_diff>

<commit_message>
Switching regulator to reduce heat, and added ground planes
</commit_message>
<xml_diff>
--- a/BOM MAIN BOARD.xlsx
+++ b/BOM MAIN BOARD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\braed\Documents\EAGLE\projects\SP Throttle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B4EA28E-10A7-4805-8BA5-CA273F005A4D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E85270E5-52AE-4B41-8369-483C84BDB6F5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2220" yWindow="2064" windowWidth="17280" windowHeight="9024" xr2:uid="{7A6408F3-8FEB-416E-8A51-1ABFD5653230}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="157">
   <si>
     <t>Qty</t>
   </si>
@@ -60,9 +60,6 @@
     <t>C0402</t>
   </si>
   <si>
-    <t>CAPACITOR, American symbol</t>
-  </si>
-  <si>
     <t>10118194-0001LF</t>
   </si>
   <si>
@@ -87,9 +84,6 @@
     <t>R4, R5, R10, R14</t>
   </si>
   <si>
-    <t>RESISTOR, American symbol</t>
-  </si>
-  <si>
     <t>1M</t>
   </si>
   <si>
@@ -99,30 +93,12 @@
     <t>1k</t>
   </si>
   <si>
-    <t>R1, R2, R3, R6, R15, R18</t>
-  </si>
-  <si>
     <t>1uf</t>
   </si>
   <si>
     <t>C3, C15</t>
   </si>
   <si>
-    <t>2.2uF</t>
-  </si>
-  <si>
-    <t>CPOL-USCT3216</t>
-  </si>
-  <si>
-    <t>CT3216</t>
-  </si>
-  <si>
-    <t>C1, C16</t>
-  </si>
-  <si>
-    <t>POLARIZED CAPACITOR, American symbol</t>
-  </si>
-  <si>
     <t>4.7k</t>
   </si>
   <si>
@@ -132,21 +108,12 @@
     <t>4.7uf</t>
   </si>
   <si>
-    <t>C9</t>
-  </si>
-  <si>
     <t>404R10KL1.0</t>
   </si>
   <si>
     <t>PT1</t>
   </si>
   <si>
-    <t>470pf</t>
-  </si>
-  <si>
-    <t>C8, C13</t>
-  </si>
-  <si>
     <t>6.8pf</t>
   </si>
   <si>
@@ -288,27 +255,6 @@
     <t>Diode</t>
   </si>
   <si>
-    <t>MIC5219-3.3YM5</t>
-  </si>
-  <si>
-    <t>MIC5219XX</t>
-  </si>
-  <si>
-    <t>SOT23-5</t>
-  </si>
-  <si>
-    <t>IC6</t>
-  </si>
-  <si>
-    <t>VOLTAGE REGULATOR</t>
-  </si>
-  <si>
-    <t>MIC5219-5.0YM5</t>
-  </si>
-  <si>
-    <t>IC7</t>
-  </si>
-  <si>
     <t>PRTR5V0U2X,215</t>
   </si>
   <si>
@@ -351,12 +297,6 @@
     <t>GRM155R61E105KA12D‎</t>
   </si>
   <si>
-    <t>TAJA225K020RNJ‎</t>
-  </si>
-  <si>
-    <t>‎GRM1555C1E471JA01D‎</t>
-  </si>
-  <si>
     <t>‎RC0402JR-074K7L</t>
   </si>
   <si>
@@ -372,9 +312,6 @@
     <t>BC817-25LT1</t>
   </si>
   <si>
-    <t xml:space="preserve">	BLM18PG471SN1D</t>
-  </si>
-  <si>
     <t>‎LTST-C191TBKT‎</t>
   </si>
   <si>
@@ -387,9 +324,6 @@
     <t>Vibrating Mini Motor Disc</t>
   </si>
   <si>
-    <t>C5, C6, C7, C10, C11, C12, C14, C17</t>
-  </si>
-  <si>
     <t>JST SH 1MM VERT</t>
   </si>
   <si>
@@ -430,13 +364,151 @@
   </si>
   <si>
     <t>CONN SOCKET 22-30AWG CRIMP GOLD</t>
+  </si>
+  <si>
+    <t>R2, R3, R15, R18</t>
+  </si>
+  <si>
+    <t>10uf</t>
+  </si>
+  <si>
+    <t>C21</t>
+  </si>
+  <si>
+    <t>C5, C6, C7, C10, C11, C12, C14, C17, C20</t>
+  </si>
+  <si>
+    <t>C1, C8, C9</t>
+  </si>
+  <si>
+    <t>22uf</t>
+  </si>
+  <si>
+    <t>C18, C19</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>4.7uH</t>
+  </si>
+  <si>
+    <t>L1812</t>
+  </si>
+  <si>
+    <t>INDUCTOR</t>
+  </si>
+  <si>
+    <t>FIXED IND 4.7UH 1.6A 90 MOHM SMD</t>
+  </si>
+  <si>
+    <t>LQH43PN4R7M26L‎</t>
+  </si>
+  <si>
+    <t>IC5</t>
+  </si>
+  <si>
+    <t>IC8</t>
+  </si>
+  <si>
+    <t>‎AP2114H-3.3TRG1‎</t>
+  </si>
+  <si>
+    <t>IC REG LINEAR 3.3V 1A SOT223</t>
+  </si>
+  <si>
+    <t>SOT223</t>
+  </si>
+  <si>
+    <t>3.3V REGULATOR</t>
+  </si>
+  <si>
+    <t>5V REGULATOR</t>
+  </si>
+  <si>
+    <t>‎AP63205WU-7‎</t>
+  </si>
+  <si>
+    <t>IC REG BUCK 5V 2A TSOT26</t>
+  </si>
+  <si>
+    <t>TSOT26</t>
+  </si>
+  <si>
+    <t>ALTIMETER</t>
+  </si>
+  <si>
+    <t>IC MOTOR DRIVER 2V-5.5V 10VSSOP</t>
+  </si>
+  <si>
+    <t>CONN RCPT 10POS 0.1 GOLD SMD R/A</t>
+  </si>
+  <si>
+    <t>FERRITE BEAD 470 OHM 0603 1LN</t>
+  </si>
+  <si>
+    <t>‎TMK212BBJ106KG-T‎</t>
+  </si>
+  <si>
+    <t>C0805</t>
+  </si>
+  <si>
+    <t>C-USC0805</t>
+  </si>
+  <si>
+    <t>CAP CER 10UF 25V X5R 0805</t>
+  </si>
+  <si>
+    <t>RES SMD 1K OHM 5% 1/16W 0402</t>
+  </si>
+  <si>
+    <t>RES SMD 10K OHM 5% 1/16W 0402</t>
+  </si>
+  <si>
+    <t>RES SMD 4.7K OHM 5% 1/16W 0402</t>
+  </si>
+  <si>
+    <t>RES SMD 1M OHM 5% 1/16W 0402</t>
+  </si>
+  <si>
+    <t>CAP CER 6.8PF 25V C0G/NP0 0402</t>
+  </si>
+  <si>
+    <t>CAP CER 1UF 25V X5R 0402</t>
+  </si>
+  <si>
+    <t>CAP CER 0.1UF 25V X6S 0402</t>
+  </si>
+  <si>
+    <t>CAP CER 4.7UF 10V X5R 0402</t>
+  </si>
+  <si>
+    <t>CAP CER 22UF 10V X5R 0603</t>
+  </si>
+  <si>
+    <t>C0603</t>
+  </si>
+  <si>
+    <t>‎GRM188R61A226ME15D‎</t>
+  </si>
+  <si>
+    <t>POT SENSOR LINEAR 12.7MM SLD TURRET</t>
+  </si>
+  <si>
+    <t>SWITCH TACTILE SPST-NO 0.05A 32V</t>
+  </si>
+  <si>
+    <t>CONN HEADER VERT 10POS 1.27MM</t>
+  </si>
+  <si>
+    <t>CABLE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -448,6 +520,12 @@
       <sz val="11"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -797,10 +875,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A2FCF1E-2965-4CA3-9C3D-EDB553ECE1A4}">
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -834,7 +912,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>101</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -842,30 +920,30 @@
         <v>2</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>28</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>29</v>
+        <v>146</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>7</v>
@@ -874,21 +952,21 @@
         <v>8</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>9</v>
+        <v>147</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>110</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>7</v>
@@ -896,22 +974,22 @@
       <c r="D4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="4">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>24</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="4">
-        <v>6</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>6</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>7</v>
@@ -920,59 +998,59 @@
         <v>8</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>9</v>
+        <v>149</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
+        <v>1</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="4">
         <v>2</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="4">
-        <v>1</v>
-      </c>
       <c r="B7" s="4" t="s">
-        <v>32</v>
+        <v>116</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>8</v>
+        <v>151</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>33</v>
+        <v>117</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>9</v>
+        <v>150</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>109</v>
+        <v>152</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -980,22 +1058,22 @@
         <v>1</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -1003,43 +1081,45 @@
         <v>1</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>1</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="F10" s="5"/>
+        <v>39</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>137</v>
+      </c>
       <c r="G10" s="3" t="s">
-        <v>113</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -1047,43 +1127,45 @@
         <v>1</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>121</v>
+        <v>99</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>121</v>
+        <v>99</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>122</v>
+        <v>100</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>120</v>
+        <v>98</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>119</v>
+        <v>97</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>1</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="F12" s="5"/>
+        <v>66</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>136</v>
+      </c>
       <c r="G12" s="3" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
@@ -1091,22 +1173,22 @@
         <v>1</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>111</v>
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -1114,20 +1196,22 @@
         <v>1</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="F14" s="5"/>
+        <v>46</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>134</v>
+      </c>
       <c r="G14" s="4" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -1135,43 +1219,45 @@
         <v>1</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>1</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="F16" s="5"/>
+        <v>56</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>135</v>
+      </c>
       <c r="G16" s="3" t="s">
-        <v>115</v>
+        <v>94</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
@@ -1179,45 +1265,45 @@
         <v>1</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>85</v>
+        <v>131</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>86</v>
+        <v>130</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>87</v>
+        <v>133</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>88</v>
+        <v>124</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>89</v>
+        <v>132</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>1</v>
       </c>
-      <c r="B18" s="4" t="s">
-        <v>90</v>
+      <c r="B18" s="3" t="s">
+        <v>126</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>86</v>
+        <v>129</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>87</v>
+        <v>128</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>91</v>
+        <v>125</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>89</v>
+        <v>127</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>90</v>
+        <v>126</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -1225,45 +1311,45 @@
         <v>1</v>
       </c>
       <c r="B19" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D19" s="4" t="s">
+      <c r="E19" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="F19" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F19" s="5" t="s">
-        <v>13</v>
-      </c>
       <c r="G19" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <v>1</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>96</v>
+        <v>119</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>52</v>
+        <v>121</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>53</v>
+        <v>120</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>97</v>
+        <v>118</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>55</v>
+        <v>122</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
@@ -1271,330 +1357,375 @@
         <v>1</v>
       </c>
       <c r="B21" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="4">
+        <v>1</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A23" s="4">
+        <v>1</v>
+      </c>
+      <c r="B23" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C23" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D23" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="E23" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="F23" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="F21" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A22" s="4">
-        <v>1</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="4">
-        <v>2</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="G23" s="4">
-        <v>1201</v>
+      <c r="G23" s="3" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>34</v>
+        <v>80</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>34</v>
+        <v>80</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>34</v>
+        <v>80</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F24" s="5"/>
-      <c r="G24" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="G24" s="4">
+        <v>1201</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="4">
         <v>1</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>47</v>
+        <v>153</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>112</v>
+        <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="4">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G26" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="4">
         <v>4</v>
       </c>
       <c r="B27" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C27" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="D27" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D27" s="4" t="s">
-        <v>16</v>
-      </c>
       <c r="E27" s="4" t="s">
-        <v>17</v>
+        <v>111</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>18</v>
+        <v>142</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="4">
         <v>4</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="C28" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D28" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="E28" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E28" s="4" t="s">
-        <v>31</v>
-      </c>
       <c r="F28" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A29" s="4">
+        <v>4</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A30" s="4">
+        <v>1</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E30" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G28" s="4" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="4">
-        <v>1</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F29" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="4">
-        <v>1</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="F30" s="5"/>
-      <c r="G30" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F30" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="4">
         <v>1</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="F31" s="5"/>
+        <v>64</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>154</v>
+      </c>
       <c r="G31" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="4">
         <v>1</v>
       </c>
       <c r="B32" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E32" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C32" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>70</v>
-      </c>
       <c r="F32" s="5" t="s">
-        <v>71</v>
+        <v>155</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="4">
-        <v>6</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="G33" t="s">
-        <v>123</v>
+        <v>1</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" s="4">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>156</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>129</v>
+        <v>106</v>
       </c>
       <c r="G34" t="s">
-        <v>124</v>
+        <v>101</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A35" s="4">
         <v>1</v>
       </c>
+      <c r="E35" s="4" t="s">
+        <v>156</v>
+      </c>
       <c r="F35" s="2" t="s">
-        <v>130</v>
+        <v>107</v>
       </c>
       <c r="G35" t="s">
-        <v>125</v>
+        <v>102</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A36" s="4">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>156</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>131</v>
+        <v>108</v>
       </c>
       <c r="G36" t="s">
-        <v>126</v>
+        <v>103</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" s="4">
+        <v>2</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="G37" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A38" s="4">
         <v>8</v>
       </c>
-      <c r="F37" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="G37" t="s">
-        <v>127</v>
+      <c r="E38" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G38" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G32">
-    <sortCondition ref="E2:E32"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G33">
+    <sortCondition ref="E2:E33"/>
   </sortState>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Rx and Tx to pin 37 and 38; Shifted location of JST; Added holes for zip tie
</commit_message>
<xml_diff>
--- a/BOM MAIN BOARD.xlsx
+++ b/BOM MAIN BOARD.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\braed\Documents\EAGLE\projects\SP Throttle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E85270E5-52AE-4B41-8369-483C84BDB6F5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D012DCB1-3B24-482D-9C05-1BC79C586776}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2220" yWindow="2064" windowWidth="17280" windowHeight="9024" xr2:uid="{7A6408F3-8FEB-416E-8A51-1ABFD5653230}"/>
+    <workbookView xWindow="0" yWindow="4440" windowWidth="13824" windowHeight="6000" xr2:uid="{7A6408F3-8FEB-416E-8A51-1ABFD5653230}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -366,9 +366,6 @@
     <t>CONN SOCKET 22-30AWG CRIMP GOLD</t>
   </si>
   <si>
-    <t>R2, R3, R15, R18</t>
-  </si>
-  <si>
     <t>10uf</t>
   </si>
   <si>
@@ -502,6 +499,9 @@
   </si>
   <si>
     <t>CABLE</t>
+  </si>
+  <si>
+    <t>R1, R2, R3, R15, R18</t>
   </si>
 </sst>
 </file>
@@ -877,8 +877,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A2FCF1E-2965-4CA3-9C3D-EDB553ECE1A4}">
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -932,7 +932,7 @@
         <v>28</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>90</v>
@@ -955,7 +955,7 @@
         <v>21</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>87</v>
@@ -975,10 +975,10 @@
         <v>8</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>82</v>
@@ -998,10 +998,10 @@
         <v>8</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>89</v>
@@ -1012,22 +1012,22 @@
         <v>1</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="F6" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>141</v>
-      </c>
       <c r="G6" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -1035,22 +1035,22 @@
         <v>2</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D7" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="G7" s="4" t="s">
         <v>151</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -1116,7 +1116,7 @@
         <v>39</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>37</v>
@@ -1162,7 +1162,7 @@
         <v>66</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>65</v>
@@ -1208,7 +1208,7 @@
         <v>46</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>45</v>
@@ -1254,7 +1254,7 @@
         <v>56</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>94</v>
@@ -1265,22 +1265,22 @@
         <v>1</v>
       </c>
       <c r="B17" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="F17" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="G17" s="3" t="s">
         <v>130</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -1288,22 +1288,22 @@
         <v>1</v>
       </c>
       <c r="B18" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="F18" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="E18" s="4" t="s">
+      <c r="G18" s="3" t="s">
         <v>125</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -1334,22 +1334,22 @@
         <v>1</v>
       </c>
       <c r="B20" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D20" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="E20" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="F20" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="D20" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="F20" s="5" t="s">
+      <c r="G20" s="3" t="s">
         <v>122</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
@@ -1461,7 +1461,7 @@
         <v>26</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G25" s="3" t="s">
         <v>25</v>
@@ -1492,7 +1492,7 @@
     </row>
     <row r="27" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>19</v>
@@ -1504,10 +1504,10 @@
         <v>15</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>111</v>
+        <v>156</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G27" s="4" t="s">
         <v>86</v>
@@ -1530,7 +1530,7 @@
         <v>16</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G28" s="4" t="s">
         <v>84</v>
@@ -1553,7 +1553,7 @@
         <v>23</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G29" s="4" t="s">
         <v>88</v>
@@ -1576,7 +1576,7 @@
         <v>18</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G30" s="4" t="s">
         <v>85</v>
@@ -1599,7 +1599,7 @@
         <v>64</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G31" s="3" t="s">
         <v>61</v>
@@ -1622,7 +1622,7 @@
         <v>68</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G32" s="3" t="s">
         <v>67</v>
@@ -1656,7 +1656,7 @@
         <v>6</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>106</v>
@@ -1670,7 +1670,7 @@
         <v>1</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F35" s="2" t="s">
         <v>107</v>
@@ -1684,7 +1684,7 @@
         <v>1</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F36" s="2" t="s">
         <v>108</v>
@@ -1698,7 +1698,7 @@
         <v>2</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F37" s="2" t="s">
         <v>109</v>
@@ -1712,7 +1712,7 @@
         <v>8</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>110</v>

</xml_diff>